<commit_message>
he terminado de comparar LSWI y NDWI en una grafica
</commit_message>
<xml_diff>
--- a/Google Earth Engine/NDWI_zones_hum_buf.xlsx
+++ b/Google Earth Engine/NDWI_zones_hum_buf.xlsx
@@ -1220,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117:E139"/>
+    <sheetView tabSelected="1" topLeftCell="A381" workbookViewId="0">
+      <selection activeCell="F312" sqref="F312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6945,6 +6945,12 @@
       <c r="C140" t="s">
         <v>6</v>
       </c>
+      <c r="D140">
+        <v>1999</v>
+      </c>
+      <c r="E140">
+        <v>-0.108839189331926</v>
+      </c>
       <c r="F140" t="s">
         <v>77</v>
       </c>
@@ -6980,6 +6986,12 @@
       <c r="C141" t="s">
         <v>6</v>
       </c>
+      <c r="D141">
+        <v>2000</v>
+      </c>
+      <c r="E141">
+        <v>-0.13184307928308001</v>
+      </c>
       <c r="F141" t="s">
         <v>77</v>
       </c>
@@ -7015,6 +7027,12 @@
       <c r="C142" t="s">
         <v>6</v>
       </c>
+      <c r="D142">
+        <v>2001</v>
+      </c>
+      <c r="E142">
+        <v>-0.105976739432634</v>
+      </c>
       <c r="F142" t="s">
         <v>77</v>
       </c>
@@ -7050,6 +7068,12 @@
       <c r="C143" t="s">
         <v>6</v>
       </c>
+      <c r="D143">
+        <v>2002</v>
+      </c>
+      <c r="E143">
+        <v>-0.107912501730624</v>
+      </c>
       <c r="F143" t="s">
         <v>77</v>
       </c>
@@ -7085,6 +7109,12 @@
       <c r="C144" t="s">
         <v>6</v>
       </c>
+      <c r="D144">
+        <v>2003</v>
+      </c>
+      <c r="E144">
+        <v>-9.0664592500789301E-2</v>
+      </c>
       <c r="F144" t="s">
         <v>77</v>
       </c>
@@ -7120,6 +7150,12 @@
       <c r="C145" t="s">
         <v>6</v>
       </c>
+      <c r="D145">
+        <v>2004</v>
+      </c>
+      <c r="E145">
+        <v>-0.124154193298701</v>
+      </c>
       <c r="F145" t="s">
         <v>77</v>
       </c>
@@ -7155,6 +7191,12 @@
       <c r="C146" t="s">
         <v>6</v>
       </c>
+      <c r="D146">
+        <v>2005</v>
+      </c>
+      <c r="E146">
+        <v>-0.102711123666733</v>
+      </c>
       <c r="F146" t="s">
         <v>77</v>
       </c>
@@ -7190,6 +7232,12 @@
       <c r="C147" t="s">
         <v>6</v>
       </c>
+      <c r="D147">
+        <v>2006</v>
+      </c>
+      <c r="E147">
+        <v>-0.114167922163906</v>
+      </c>
       <c r="F147" t="s">
         <v>77</v>
       </c>
@@ -7225,6 +7273,12 @@
       <c r="C148" t="s">
         <v>6</v>
       </c>
+      <c r="D148">
+        <v>2007</v>
+      </c>
+      <c r="E148">
+        <v>-0.13368530956678401</v>
+      </c>
       <c r="F148" t="s">
         <v>77</v>
       </c>
@@ -7260,6 +7314,12 @@
       <c r="C149" t="s">
         <v>6</v>
       </c>
+      <c r="D149">
+        <v>2008</v>
+      </c>
+      <c r="E149">
+        <v>-0.112305512280229</v>
+      </c>
       <c r="F149" t="s">
         <v>77</v>
       </c>
@@ -7295,6 +7355,12 @@
       <c r="C150" t="s">
         <v>6</v>
       </c>
+      <c r="D150">
+        <v>2009</v>
+      </c>
+      <c r="E150">
+        <v>-0.135696116288515</v>
+      </c>
       <c r="F150" t="s">
         <v>77</v>
       </c>
@@ -7330,6 +7396,12 @@
       <c r="C151" t="s">
         <v>6</v>
       </c>
+      <c r="D151">
+        <v>2010</v>
+      </c>
+      <c r="E151">
+        <v>-0.14934041252809199</v>
+      </c>
       <c r="F151" t="s">
         <v>77</v>
       </c>
@@ -7365,6 +7437,12 @@
       <c r="C152" t="s">
         <v>6</v>
       </c>
+      <c r="D152">
+        <v>2011</v>
+      </c>
+      <c r="E152">
+        <v>-0.105870608827893</v>
+      </c>
       <c r="F152" t="s">
         <v>77</v>
       </c>
@@ -7400,6 +7478,12 @@
       <c r="C153" t="s">
         <v>6</v>
       </c>
+      <c r="D153">
+        <v>2012</v>
+      </c>
+      <c r="E153">
+        <v>-0.11425575227368399</v>
+      </c>
       <c r="F153" t="s">
         <v>77</v>
       </c>
@@ -7435,6 +7519,12 @@
       <c r="C154" t="s">
         <v>6</v>
       </c>
+      <c r="D154">
+        <v>2013</v>
+      </c>
+      <c r="E154">
+        <v>-0.12804877038314799</v>
+      </c>
       <c r="F154" t="s">
         <v>77</v>
       </c>
@@ -7470,6 +7560,12 @@
       <c r="C155" t="s">
         <v>6</v>
       </c>
+      <c r="D155">
+        <v>2014</v>
+      </c>
+      <c r="E155">
+        <v>-0.12796737824562801</v>
+      </c>
       <c r="F155" t="s">
         <v>77</v>
       </c>
@@ -7505,6 +7601,12 @@
       <c r="C156" t="s">
         <v>6</v>
       </c>
+      <c r="D156">
+        <v>2015</v>
+      </c>
+      <c r="E156">
+        <v>-0.116187983768672</v>
+      </c>
       <c r="F156" t="s">
         <v>77</v>
       </c>
@@ -7540,6 +7642,12 @@
       <c r="C157" t="s">
         <v>6</v>
       </c>
+      <c r="D157">
+        <v>2016</v>
+      </c>
+      <c r="E157">
+        <v>-0.10247965699244201</v>
+      </c>
       <c r="F157" t="s">
         <v>77</v>
       </c>
@@ -7575,6 +7683,12 @@
       <c r="C158" t="s">
         <v>6</v>
       </c>
+      <c r="D158">
+        <v>2017</v>
+      </c>
+      <c r="E158">
+        <v>-0.104463509249538</v>
+      </c>
       <c r="F158" t="s">
         <v>77</v>
       </c>
@@ -7610,6 +7724,12 @@
       <c r="C159" t="s">
         <v>6</v>
       </c>
+      <c r="D159">
+        <v>2018</v>
+      </c>
+      <c r="E159">
+        <v>-0.108817340595651</v>
+      </c>
       <c r="F159" t="s">
         <v>77</v>
       </c>
@@ -7645,6 +7765,12 @@
       <c r="C160" t="s">
         <v>6</v>
       </c>
+      <c r="D160">
+        <v>2019</v>
+      </c>
+      <c r="E160">
+        <v>-0.12594087121427699</v>
+      </c>
       <c r="F160" t="s">
         <v>77</v>
       </c>
@@ -7680,6 +7806,12 @@
       <c r="C161" t="s">
         <v>6</v>
       </c>
+      <c r="D161">
+        <v>2020</v>
+      </c>
+      <c r="E161">
+        <v>-0.122098814587754</v>
+      </c>
       <c r="F161" t="s">
         <v>77</v>
       </c>
@@ -7715,6 +7847,12 @@
       <c r="C162" t="s">
         <v>6</v>
       </c>
+      <c r="D162">
+        <v>2021</v>
+      </c>
+      <c r="E162">
+        <v>-0.11426762032085901</v>
+      </c>
       <c r="F162" t="s">
         <v>77</v>
       </c>
@@ -7750,6 +7888,12 @@
       <c r="C163" t="s">
         <v>6</v>
       </c>
+      <c r="D163">
+        <v>1999</v>
+      </c>
+      <c r="E163">
+        <v>-9.27959741394528E-2</v>
+      </c>
       <c r="F163" t="s">
         <v>75</v>
       </c>
@@ -7785,6 +7929,12 @@
       <c r="C164" t="s">
         <v>6</v>
       </c>
+      <c r="D164">
+        <v>2000</v>
+      </c>
+      <c r="E164">
+        <v>-9.0883974157203604E-2</v>
+      </c>
       <c r="F164" t="s">
         <v>75</v>
       </c>
@@ -7820,6 +7970,12 @@
       <c r="C165" t="s">
         <v>6</v>
       </c>
+      <c r="D165">
+        <v>2001</v>
+      </c>
+      <c r="E165">
+        <v>-9.2498682418718906E-2</v>
+      </c>
       <c r="F165" t="s">
         <v>75</v>
       </c>
@@ -7855,6 +8011,12 @@
       <c r="C166" t="s">
         <v>6</v>
       </c>
+      <c r="D166">
+        <v>2002</v>
+      </c>
+      <c r="E166">
+        <v>-8.6813909659085503E-2</v>
+      </c>
       <c r="F166" t="s">
         <v>75</v>
       </c>
@@ -7890,6 +8052,12 @@
       <c r="C167" t="s">
         <v>6</v>
       </c>
+      <c r="D167">
+        <v>2003</v>
+      </c>
+      <c r="E167">
+        <v>-8.6765315006635604E-2</v>
+      </c>
       <c r="F167" t="s">
         <v>75</v>
       </c>
@@ -7925,6 +8093,12 @@
       <c r="C168" t="s">
         <v>6</v>
       </c>
+      <c r="D168">
+        <v>2004</v>
+      </c>
+      <c r="E168">
+        <v>-0.100471445242284</v>
+      </c>
       <c r="F168" t="s">
         <v>75</v>
       </c>
@@ -7960,6 +8134,12 @@
       <c r="C169" t="s">
         <v>6</v>
       </c>
+      <c r="D169">
+        <v>2005</v>
+      </c>
+      <c r="E169">
+        <v>-9.4822406174482898E-2</v>
+      </c>
       <c r="F169" t="s">
         <v>75</v>
       </c>
@@ -7995,6 +8175,12 @@
       <c r="C170" t="s">
         <v>6</v>
       </c>
+      <c r="D170">
+        <v>2006</v>
+      </c>
+      <c r="E170">
+        <v>-9.8615292587056702E-2</v>
+      </c>
       <c r="F170" t="s">
         <v>75</v>
       </c>
@@ -8030,6 +8216,12 @@
       <c r="C171" t="s">
         <v>6</v>
       </c>
+      <c r="D171">
+        <v>2007</v>
+      </c>
+      <c r="E171">
+        <v>-9.86500573026943E-2</v>
+      </c>
       <c r="F171" t="s">
         <v>75</v>
       </c>
@@ -8065,6 +8257,12 @@
       <c r="C172" t="s">
         <v>6</v>
       </c>
+      <c r="D172">
+        <v>2008</v>
+      </c>
+      <c r="E172">
+        <v>-0.10452524102651101</v>
+      </c>
       <c r="F172" t="s">
         <v>75</v>
       </c>
@@ -8100,6 +8298,12 @@
       <c r="C173" t="s">
         <v>6</v>
       </c>
+      <c r="D173">
+        <v>2009</v>
+      </c>
+      <c r="E173">
+        <v>-0.100411191582679</v>
+      </c>
       <c r="F173" t="s">
         <v>75</v>
       </c>
@@ -8135,6 +8339,12 @@
       <c r="C174" t="s">
         <v>6</v>
       </c>
+      <c r="D174">
+        <v>2010</v>
+      </c>
+      <c r="E174">
+        <v>-0.116069675190242</v>
+      </c>
       <c r="F174" t="s">
         <v>75</v>
       </c>
@@ -8170,6 +8380,12 @@
       <c r="C175" t="s">
         <v>6</v>
       </c>
+      <c r="D175">
+        <v>2011</v>
+      </c>
+      <c r="E175">
+        <v>-0.108699941274347</v>
+      </c>
       <c r="F175" t="s">
         <v>75</v>
       </c>
@@ -8205,6 +8421,12 @@
       <c r="C176" t="s">
         <v>6</v>
       </c>
+      <c r="D176">
+        <v>2012</v>
+      </c>
+      <c r="E176">
+        <v>-0.10257039121183199</v>
+      </c>
       <c r="F176" t="s">
         <v>75</v>
       </c>
@@ -8240,6 +8462,12 @@
       <c r="C177" t="s">
         <v>6</v>
       </c>
+      <c r="D177">
+        <v>2013</v>
+      </c>
+      <c r="E177">
+        <v>-0.110198965773549</v>
+      </c>
       <c r="F177" t="s">
         <v>75</v>
       </c>
@@ -8275,6 +8503,12 @@
       <c r="C178" t="s">
         <v>6</v>
       </c>
+      <c r="D178">
+        <v>2014</v>
+      </c>
+      <c r="E178">
+        <v>-0.106486666127594</v>
+      </c>
       <c r="F178" t="s">
         <v>75</v>
       </c>
@@ -8310,6 +8544,12 @@
       <c r="C179" t="s">
         <v>6</v>
       </c>
+      <c r="D179">
+        <v>2015</v>
+      </c>
+      <c r="E179">
+        <v>-0.106325078478347</v>
+      </c>
       <c r="F179" t="s">
         <v>75</v>
       </c>
@@ -8345,6 +8585,12 @@
       <c r="C180" t="s">
         <v>6</v>
       </c>
+      <c r="D180">
+        <v>2016</v>
+      </c>
+      <c r="E180">
+        <v>-0.112478539370165</v>
+      </c>
       <c r="F180" t="s">
         <v>75</v>
       </c>
@@ -8380,6 +8626,12 @@
       <c r="C181" t="s">
         <v>6</v>
       </c>
+      <c r="D181">
+        <v>2017</v>
+      </c>
+      <c r="E181">
+        <v>-0.108482050999688</v>
+      </c>
       <c r="F181" t="s">
         <v>75</v>
       </c>
@@ -8415,6 +8667,12 @@
       <c r="C182" t="s">
         <v>6</v>
       </c>
+      <c r="D182">
+        <v>2018</v>
+      </c>
+      <c r="E182">
+        <v>-0.106407249701213</v>
+      </c>
       <c r="F182" t="s">
         <v>75</v>
       </c>
@@ -8450,6 +8708,12 @@
       <c r="C183" t="s">
         <v>6</v>
       </c>
+      <c r="D183">
+        <v>2019</v>
+      </c>
+      <c r="E183">
+        <v>-0.106329380017659</v>
+      </c>
       <c r="F183" t="s">
         <v>75</v>
       </c>
@@ -8485,6 +8749,12 @@
       <c r="C184" t="s">
         <v>6</v>
       </c>
+      <c r="D184">
+        <v>2020</v>
+      </c>
+      <c r="E184">
+        <v>-0.10445414243913501</v>
+      </c>
       <c r="F184" t="s">
         <v>75</v>
       </c>
@@ -8520,6 +8790,12 @@
       <c r="C185" t="s">
         <v>6</v>
       </c>
+      <c r="D185">
+        <v>2021</v>
+      </c>
+      <c r="E185">
+        <v>-0.100719788811688</v>
+      </c>
       <c r="F185" t="s">
         <v>75</v>
       </c>
@@ -8555,6 +8831,12 @@
       <c r="C186" t="s">
         <v>6</v>
       </c>
+      <c r="D186">
+        <v>1999</v>
+      </c>
+      <c r="E186">
+        <v>-7.66291846113933E-2</v>
+      </c>
       <c r="F186" t="s">
         <v>74</v>
       </c>
@@ -8590,6 +8872,12 @@
       <c r="C187" t="s">
         <v>6</v>
       </c>
+      <c r="D187">
+        <v>2000</v>
+      </c>
+      <c r="E187">
+        <v>-8.04686288051496E-2</v>
+      </c>
       <c r="F187" t="s">
         <v>74</v>
       </c>
@@ -8625,6 +8913,12 @@
       <c r="C188" t="s">
         <v>6</v>
       </c>
+      <c r="D188">
+        <v>2001</v>
+      </c>
+      <c r="E188">
+        <v>-8.8825811090478601E-2</v>
+      </c>
       <c r="F188" t="s">
         <v>74</v>
       </c>
@@ -8660,6 +8954,12 @@
       <c r="C189" t="s">
         <v>6</v>
       </c>
+      <c r="D189">
+        <v>2002</v>
+      </c>
+      <c r="E189">
+        <v>-8.6370431667189301E-2</v>
+      </c>
       <c r="F189" t="s">
         <v>74</v>
       </c>
@@ -8695,6 +8995,12 @@
       <c r="C190" t="s">
         <v>6</v>
       </c>
+      <c r="D190">
+        <v>2003</v>
+      </c>
+      <c r="E190">
+        <v>-9.8705625289226495E-2</v>
+      </c>
       <c r="F190" t="s">
         <v>74</v>
       </c>
@@ -8730,6 +9036,12 @@
       <c r="C191" t="s">
         <v>6</v>
       </c>
+      <c r="D191">
+        <v>2004</v>
+      </c>
+      <c r="E191">
+        <v>-0.100594265396826</v>
+      </c>
       <c r="F191" t="s">
         <v>74</v>
       </c>
@@ -8765,6 +9077,12 @@
       <c r="C192" t="s">
         <v>6</v>
       </c>
+      <c r="D192">
+        <v>2005</v>
+      </c>
+      <c r="E192">
+        <v>-0.10056848467709199</v>
+      </c>
       <c r="F192" t="s">
         <v>74</v>
       </c>
@@ -8800,6 +9118,12 @@
       <c r="C193" t="s">
         <v>6</v>
       </c>
+      <c r="D193">
+        <v>2006</v>
+      </c>
+      <c r="E193">
+        <v>-9.8641995843064795E-2</v>
+      </c>
       <c r="F193" t="s">
         <v>74</v>
       </c>
@@ -8835,6 +9159,12 @@
       <c r="C194" t="s">
         <v>6</v>
       </c>
+      <c r="D194">
+        <v>2007</v>
+      </c>
+      <c r="E194">
+        <v>-9.0873844131299703E-2</v>
+      </c>
       <c r="F194" t="s">
         <v>74</v>
       </c>
@@ -8870,6 +9200,12 @@
       <c r="C195" t="s">
         <v>6</v>
       </c>
+      <c r="D195">
+        <v>2008</v>
+      </c>
+      <c r="E195">
+        <v>-9.8608185879070498E-2</v>
+      </c>
       <c r="F195" t="s">
         <v>74</v>
       </c>
@@ -8905,6 +9241,12 @@
       <c r="C196" t="s">
         <v>6</v>
       </c>
+      <c r="D196">
+        <v>2009</v>
+      </c>
+      <c r="E196">
+        <v>-9.2803284302511502E-2</v>
+      </c>
       <c r="F196" t="s">
         <v>74</v>
       </c>
@@ -8940,6 +9282,12 @@
       <c r="C197" t="s">
         <v>6</v>
       </c>
+      <c r="D197">
+        <v>2010</v>
+      </c>
+      <c r="E197">
+        <v>-0.104467713979156</v>
+      </c>
       <c r="F197" t="s">
         <v>74</v>
       </c>
@@ -8975,6 +9323,12 @@
       <c r="C198" t="s">
         <v>6</v>
       </c>
+      <c r="D198">
+        <v>2011</v>
+      </c>
+      <c r="E198">
+        <v>-0.104418079336085</v>
+      </c>
       <c r="F198" t="s">
         <v>74</v>
       </c>
@@ -9010,6 +9364,12 @@
       <c r="C199" t="s">
         <v>6</v>
       </c>
+      <c r="D199">
+        <v>2012</v>
+      </c>
+      <c r="E199">
+        <v>-9.2720601605452105E-2</v>
+      </c>
       <c r="F199" t="s">
         <v>74</v>
       </c>
@@ -9045,6 +9405,12 @@
       <c r="C200" t="s">
         <v>6</v>
       </c>
+      <c r="D200">
+        <v>2013</v>
+      </c>
+      <c r="E200">
+        <v>-8.2993655544641304E-2</v>
+      </c>
       <c r="F200" t="s">
         <v>74</v>
       </c>
@@ -9080,6 +9446,12 @@
       <c r="C201" t="s">
         <v>6</v>
       </c>
+      <c r="D201">
+        <v>2014</v>
+      </c>
+      <c r="E201">
+        <v>-8.5018697455683107E-2</v>
+      </c>
       <c r="F201" t="s">
         <v>74</v>
       </c>
@@ -9115,6 +9487,12 @@
       <c r="C202" t="s">
         <v>6</v>
       </c>
+      <c r="D202">
+        <v>2015</v>
+      </c>
+      <c r="E202">
+        <v>-9.2780913589428499E-2</v>
+      </c>
       <c r="F202" t="s">
         <v>74</v>
       </c>
@@ -9150,6 +9528,12 @@
       <c r="C203" t="s">
         <v>6</v>
       </c>
+      <c r="D203">
+        <v>2016</v>
+      </c>
+      <c r="E203">
+        <v>-7.91566871785057E-2</v>
+      </c>
       <c r="F203" t="s">
         <v>74</v>
       </c>
@@ -9185,6 +9569,12 @@
       <c r="C204" t="s">
         <v>6</v>
       </c>
+      <c r="D204">
+        <v>2017</v>
+      </c>
+      <c r="E204">
+        <v>-9.6646548307334296E-2</v>
+      </c>
       <c r="F204" t="s">
         <v>74</v>
       </c>
@@ -9220,6 +9610,12 @@
       <c r="C205" t="s">
         <v>6</v>
       </c>
+      <c r="D205">
+        <v>2018</v>
+      </c>
+      <c r="E205">
+        <v>-9.8633047700493401E-2</v>
+      </c>
       <c r="F205" t="s">
         <v>74</v>
       </c>
@@ -9255,6 +9651,12 @@
       <c r="C206" t="s">
         <v>6</v>
       </c>
+      <c r="D206">
+        <v>2019</v>
+      </c>
+      <c r="E206">
+        <v>-8.9012690431247002E-2</v>
+      </c>
       <c r="F206" t="s">
         <v>74</v>
       </c>
@@ -9290,6 +9692,12 @@
       <c r="C207" t="s">
         <v>6</v>
       </c>
+      <c r="D207">
+        <v>2020</v>
+      </c>
+      <c r="E207">
+        <v>-8.6896332665469506E-2</v>
+      </c>
       <c r="F207" t="s">
         <v>74</v>
       </c>
@@ -9325,6 +9733,12 @@
       <c r="C208" t="s">
         <v>6</v>
       </c>
+      <c r="D208">
+        <v>2021</v>
+      </c>
+      <c r="E208">
+        <v>-8.8963750640122394E-2</v>
+      </c>
       <c r="F208" t="s">
         <v>74</v>
       </c>
@@ -9360,6 +9774,12 @@
       <c r="C209" t="s">
         <v>6</v>
       </c>
+      <c r="D209">
+        <v>1999</v>
+      </c>
+      <c r="E209">
+        <v>-5.5620989304597197E-2</v>
+      </c>
       <c r="F209" t="s">
         <v>77</v>
       </c>
@@ -9395,6 +9815,12 @@
       <c r="C210" t="s">
         <v>6</v>
       </c>
+      <c r="D210">
+        <v>2000</v>
+      </c>
+      <c r="E210">
+        <v>-5.98213233679524E-2</v>
+      </c>
       <c r="F210" t="s">
         <v>77</v>
       </c>
@@ -9430,6 +9856,12 @@
       <c r="C211" t="s">
         <v>6</v>
       </c>
+      <c r="D211">
+        <v>2001</v>
+      </c>
+      <c r="E211">
+        <v>-5.58792583126662E-2</v>
+      </c>
       <c r="F211" t="s">
         <v>77</v>
       </c>
@@ -9465,6 +9897,12 @@
       <c r="C212" t="s">
         <v>6</v>
       </c>
+      <c r="D212">
+        <v>2002</v>
+      </c>
+      <c r="E212">
+        <v>-5.71227543985139E-2</v>
+      </c>
       <c r="F212" t="s">
         <v>77</v>
       </c>
@@ -9500,6 +9938,12 @@
       <c r="C213" t="s">
         <v>6</v>
       </c>
+      <c r="D213">
+        <v>2003</v>
+      </c>
+      <c r="E213">
+        <v>-5.7586715912945202E-2</v>
+      </c>
       <c r="F213" t="s">
         <v>77</v>
       </c>
@@ -9535,6 +9979,12 @@
       <c r="C214" t="s">
         <v>6</v>
       </c>
+      <c r="D214">
+        <v>2004</v>
+      </c>
+      <c r="E214">
+        <v>-5.9752818143904103E-2</v>
+      </c>
       <c r="F214" t="s">
         <v>77</v>
       </c>
@@ -9570,6 +10020,12 @@
       <c r="C215" t="s">
         <v>6</v>
       </c>
+      <c r="D215">
+        <v>2005</v>
+      </c>
+      <c r="E215">
+        <v>-6.1474977122610498E-2</v>
+      </c>
       <c r="F215" t="s">
         <v>77</v>
       </c>
@@ -9605,6 +10061,12 @@
       <c r="C216" t="s">
         <v>6</v>
       </c>
+      <c r="D216">
+        <v>2006</v>
+      </c>
+      <c r="E216">
+        <v>-6.15457500473474E-2</v>
+      </c>
       <c r="F216" t="s">
         <v>77</v>
       </c>
@@ -9640,6 +10102,12 @@
       <c r="C217" t="s">
         <v>6</v>
       </c>
+      <c r="D217">
+        <v>2007</v>
+      </c>
+      <c r="E217">
+        <v>-5.7667949969655498E-2</v>
+      </c>
       <c r="F217" t="s">
         <v>77</v>
       </c>
@@ -9675,6 +10143,12 @@
       <c r="C218" t="s">
         <v>6</v>
       </c>
+      <c r="D218">
+        <v>2008</v>
+      </c>
+      <c r="E218">
+        <v>-5.77665198958182E-2</v>
+      </c>
       <c r="F218" t="s">
         <v>77</v>
       </c>
@@ -9710,6 +10184,12 @@
       <c r="C219" t="s">
         <v>6</v>
       </c>
+      <c r="D219">
+        <v>2009</v>
+      </c>
+      <c r="E219">
+        <v>-4.9967740035222197E-2</v>
+      </c>
       <c r="F219" t="s">
         <v>77</v>
       </c>
@@ -9745,6 +10225,12 @@
       <c r="C220" t="s">
         <v>6</v>
       </c>
+      <c r="D220">
+        <v>2010</v>
+      </c>
+      <c r="E220">
+        <v>-5.1784342006851898E-2</v>
+      </c>
       <c r="F220" t="s">
         <v>77</v>
       </c>
@@ -9780,6 +10266,12 @@
       <c r="C221" t="s">
         <v>6</v>
       </c>
+      <c r="D221">
+        <v>2011</v>
+      </c>
+      <c r="E221">
+        <v>-6.1473238691506303E-2</v>
+      </c>
       <c r="F221" t="s">
         <v>77</v>
       </c>
@@ -9815,6 +10307,12 @@
       <c r="C222" t="s">
         <v>6</v>
       </c>
+      <c r="D222">
+        <v>2012</v>
+      </c>
+      <c r="E222">
+        <v>-6.1552356747609102E-2</v>
+      </c>
       <c r="F222" t="s">
         <v>77</v>
       </c>
@@ -9850,6 +10348,12 @@
       <c r="C223" t="s">
         <v>6</v>
       </c>
+      <c r="D223">
+        <v>2013</v>
+      </c>
+      <c r="E223">
+        <v>-6.3476051454201099E-2</v>
+      </c>
       <c r="F223" t="s">
         <v>77</v>
       </c>
@@ -9885,6 +10389,12 @@
       <c r="C224" t="s">
         <v>6</v>
       </c>
+      <c r="D224">
+        <v>2014</v>
+      </c>
+      <c r="E224">
+        <v>-6.3558970416454405E-2</v>
+      </c>
       <c r="F224" t="s">
         <v>77</v>
       </c>
@@ -9920,6 +10430,12 @@
       <c r="C225" t="s">
         <v>6</v>
       </c>
+      <c r="D225">
+        <v>2015</v>
+      </c>
+      <c r="E225">
+        <v>-6.16759120464948E-2</v>
+      </c>
       <c r="F225" t="s">
         <v>77</v>
       </c>
@@ -9955,6 +10471,12 @@
       <c r="C226" t="s">
         <v>6</v>
       </c>
+      <c r="D226">
+        <v>2016</v>
+      </c>
+      <c r="E226">
+        <v>-6.1606958181640602E-2</v>
+      </c>
       <c r="F226" t="s">
         <v>77</v>
       </c>
@@ -9990,6 +10512,12 @@
       <c r="C227" t="s">
         <v>6</v>
       </c>
+      <c r="D227">
+        <v>2017</v>
+      </c>
+      <c r="E227">
+        <v>-5.7618186735104999E-2</v>
+      </c>
       <c r="F227" t="s">
         <v>77</v>
       </c>
@@ -10025,6 +10553,12 @@
       <c r="C228" t="s">
         <v>6</v>
       </c>
+      <c r="D228">
+        <v>2018</v>
+      </c>
+      <c r="E228">
+        <v>-6.3508416489693603E-2</v>
+      </c>
       <c r="F228" t="s">
         <v>77</v>
       </c>
@@ -10060,6 +10594,12 @@
       <c r="C229" t="s">
         <v>6</v>
       </c>
+      <c r="D229">
+        <v>2019</v>
+      </c>
+      <c r="E229">
+        <v>-5.5623727814110402E-2</v>
+      </c>
       <c r="F229" t="s">
         <v>77</v>
       </c>
@@ -10095,6 +10635,12 @@
       <c r="C230" t="s">
         <v>6</v>
       </c>
+      <c r="D230">
+        <v>2020</v>
+      </c>
+      <c r="E230">
+        <v>-5.9645578577238602E-2</v>
+      </c>
       <c r="F230" t="s">
         <v>77</v>
       </c>
@@ -10130,6 +10676,12 @@
       <c r="C231" t="s">
         <v>6</v>
       </c>
+      <c r="D231">
+        <v>2021</v>
+      </c>
+      <c r="E231">
+        <v>-6.3506323688839794E-2</v>
+      </c>
       <c r="F231" t="s">
         <v>77</v>
       </c>
@@ -10165,6 +10717,12 @@
       <c r="C232" t="s">
         <v>6</v>
       </c>
+      <c r="D232">
+        <v>1999</v>
+      </c>
+      <c r="E232">
+        <v>-0.11235188112880801</v>
+      </c>
       <c r="F232" t="s">
         <v>77</v>
       </c>
@@ -10200,6 +10758,12 @@
       <c r="C233" t="s">
         <v>6</v>
       </c>
+      <c r="D233">
+        <v>2000</v>
+      </c>
+      <c r="E233">
+        <v>-0.12007248165444</v>
+      </c>
       <c r="F233" t="s">
         <v>77</v>
       </c>
@@ -10235,6 +10799,12 @@
       <c r="C234" t="s">
         <v>6</v>
       </c>
+      <c r="D234">
+        <v>2001</v>
+      </c>
+      <c r="E234">
+        <v>-0.118165554864629</v>
+      </c>
       <c r="F234" t="s">
         <v>77</v>
       </c>
@@ -10270,6 +10840,12 @@
       <c r="C235" t="s">
         <v>6</v>
       </c>
+      <c r="D235">
+        <v>2002</v>
+      </c>
+      <c r="E235">
+        <v>-0.112369349612677</v>
+      </c>
       <c r="F235" t="s">
         <v>77</v>
       </c>
@@ -10305,6 +10881,12 @@
       <c r="C236" t="s">
         <v>6</v>
       </c>
+      <c r="D236">
+        <v>2003</v>
+      </c>
+      <c r="E236">
+        <v>-0.11996578992597599</v>
+      </c>
       <c r="F236" t="s">
         <v>77</v>
       </c>
@@ -10340,6 +10922,12 @@
       <c r="C237" t="s">
         <v>6</v>
       </c>
+      <c r="D237">
+        <v>2004</v>
+      </c>
+      <c r="E237">
+        <v>-0.145576662951727</v>
+      </c>
       <c r="F237" t="s">
         <v>77</v>
       </c>
@@ -10375,6 +10963,12 @@
       <c r="C238" t="s">
         <v>6</v>
       </c>
+      <c r="D238">
+        <v>2005</v>
+      </c>
+      <c r="E238">
+        <v>-0.14739000797034801</v>
+      </c>
       <c r="F238" t="s">
         <v>77</v>
       </c>
@@ -10410,6 +11004,12 @@
       <c r="C239" t="s">
         <v>6</v>
       </c>
+      <c r="D239">
+        <v>2006</v>
+      </c>
+      <c r="E239">
+        <v>-0.13176427395742099</v>
+      </c>
       <c r="F239" t="s">
         <v>77</v>
       </c>
@@ -10445,6 +11045,12 @@
       <c r="C240" t="s">
         <v>6</v>
       </c>
+      <c r="D240">
+        <v>2007</v>
+      </c>
+      <c r="E240">
+        <v>-0.13993594904047299</v>
+      </c>
       <c r="F240" t="s">
         <v>77</v>
       </c>
@@ -10480,6 +11086,12 @@
       <c r="C241" t="s">
         <v>6</v>
       </c>
+      <c r="D241">
+        <v>2008</v>
+      </c>
+      <c r="E241">
+        <v>-0.15139974722676799</v>
+      </c>
       <c r="F241" t="s">
         <v>77</v>
       </c>
@@ -10515,6 +11127,12 @@
       <c r="C242" t="s">
         <v>6</v>
       </c>
+      <c r="D242">
+        <v>2009</v>
+      </c>
+      <c r="E242">
+        <v>-0.13969163147225599</v>
+      </c>
       <c r="F242" t="s">
         <v>77</v>
       </c>
@@ -10550,6 +11168,12 @@
       <c r="C243" t="s">
         <v>6</v>
       </c>
+      <c r="D243">
+        <v>2010</v>
+      </c>
+      <c r="E243">
+        <v>-0.145485733825574</v>
+      </c>
       <c r="F243" t="s">
         <v>77</v>
       </c>
@@ -10585,6 +11209,12 @@
       <c r="C244" t="s">
         <v>6</v>
       </c>
+      <c r="D244">
+        <v>2011</v>
+      </c>
+      <c r="E244">
+        <v>-0.14153370801176901</v>
+      </c>
       <c r="F244" t="s">
         <v>77</v>
       </c>
@@ -10620,6 +11250,12 @@
       <c r="C245" t="s">
         <v>6</v>
       </c>
+      <c r="D245">
+        <v>2012</v>
+      </c>
+      <c r="E245">
+        <v>-0.153410962150794</v>
+      </c>
       <c r="F245" t="s">
         <v>77</v>
       </c>
@@ -10655,6 +11291,12 @@
       <c r="C246" t="s">
         <v>6</v>
       </c>
+      <c r="D246">
+        <v>2013</v>
+      </c>
+      <c r="E246">
+        <v>-0.12996567988873101</v>
+      </c>
       <c r="F246" t="s">
         <v>77</v>
       </c>
@@ -10690,6 +11332,12 @@
       <c r="C247" t="s">
         <v>6</v>
       </c>
+      <c r="D247">
+        <v>2014</v>
+      </c>
+      <c r="E247">
+        <v>-0.141835533003871</v>
+      </c>
       <c r="F247" t="s">
         <v>77</v>
       </c>
@@ -10725,6 +11373,12 @@
       <c r="C248" t="s">
         <v>6</v>
       </c>
+      <c r="D248">
+        <v>2015</v>
+      </c>
+      <c r="E248">
+        <v>-0.13580463252521</v>
+      </c>
       <c r="F248" t="s">
         <v>77</v>
       </c>
@@ -10760,6 +11414,12 @@
       <c r="C249" t="s">
         <v>6</v>
       </c>
+      <c r="D249">
+        <v>2016</v>
+      </c>
+      <c r="E249">
+        <v>-0.129855360265897</v>
+      </c>
       <c r="F249" t="s">
         <v>77</v>
       </c>
@@ -10795,6 +11455,12 @@
       <c r="C250" t="s">
         <v>6</v>
       </c>
+      <c r="D250">
+        <v>2017</v>
+      </c>
+      <c r="E250">
+        <v>-0.14148636091568301</v>
+      </c>
       <c r="F250" t="s">
         <v>77</v>
       </c>
@@ -10830,6 +11496,12 @@
       <c r="C251" t="s">
         <v>6</v>
       </c>
+      <c r="D251">
+        <v>2018</v>
+      </c>
+      <c r="E251">
+        <v>-0.12989947139034499</v>
+      </c>
       <c r="F251" t="s">
         <v>77</v>
       </c>
@@ -10865,6 +11537,12 @@
       <c r="C252" t="s">
         <v>6</v>
       </c>
+      <c r="D252">
+        <v>2019</v>
+      </c>
+      <c r="E252">
+        <v>-0.13572504614962599</v>
+      </c>
       <c r="F252" t="s">
         <v>77</v>
       </c>
@@ -10900,6 +11578,12 @@
       <c r="C253" t="s">
         <v>6</v>
       </c>
+      <c r="D253">
+        <v>2020</v>
+      </c>
+      <c r="E253">
+        <v>-0.12996879873766601</v>
+      </c>
       <c r="F253" t="s">
         <v>77</v>
       </c>
@@ -10935,6 +11619,12 @@
       <c r="C254" t="s">
         <v>6</v>
       </c>
+      <c r="D254">
+        <v>2021</v>
+      </c>
+      <c r="E254">
+        <v>-0.129819699239411</v>
+      </c>
       <c r="F254" t="s">
         <v>77</v>
       </c>
@@ -10970,6 +11660,12 @@
       <c r="C255" t="s">
         <v>6</v>
       </c>
+      <c r="D255">
+        <v>1999</v>
+      </c>
+      <c r="E255">
+        <v>-0.103024310376972</v>
+      </c>
       <c r="F255" t="s">
         <v>74</v>
       </c>
@@ -11005,6 +11701,12 @@
       <c r="C256" t="s">
         <v>6</v>
       </c>
+      <c r="D256">
+        <v>2000</v>
+      </c>
+      <c r="E256">
+        <v>-0.107898403603873</v>
+      </c>
       <c r="F256" t="s">
         <v>74</v>
       </c>
@@ -11040,6 +11742,12 @@
       <c r="C257" t="s">
         <v>6</v>
       </c>
+      <c r="D257">
+        <v>2001</v>
+      </c>
+      <c r="E257">
+        <v>-0.100088291499159</v>
+      </c>
       <c r="F257" t="s">
         <v>74</v>
       </c>
@@ -11075,6 +11783,12 @@
       <c r="C258" t="s">
         <v>6</v>
       </c>
+      <c r="D258">
+        <v>2002</v>
+      </c>
+      <c r="E258">
+        <v>-9.3278098492320105E-2</v>
+      </c>
       <c r="F258" t="s">
         <v>74</v>
       </c>
@@ -11110,6 +11824,12 @@
       <c r="C259" t="s">
         <v>6</v>
       </c>
+      <c r="D259">
+        <v>2003</v>
+      </c>
+      <c r="E259">
+        <v>-9.7152519452122194E-2</v>
+      </c>
       <c r="F259" t="s">
         <v>74</v>
       </c>
@@ -11145,6 +11865,12 @@
       <c r="C260" t="s">
         <v>6</v>
       </c>
+      <c r="D260">
+        <v>2004</v>
+      </c>
+      <c r="E260">
+        <v>-0.108902732543446</v>
+      </c>
       <c r="F260" t="s">
         <v>74</v>
       </c>
@@ -11180,6 +11906,12 @@
       <c r="C261" t="s">
         <v>6</v>
       </c>
+      <c r="D261">
+        <v>2005</v>
+      </c>
+      <c r="E261">
+        <v>-9.8153608265294401E-2</v>
+      </c>
       <c r="F261" t="s">
         <v>74</v>
       </c>
@@ -11215,6 +11947,12 @@
       <c r="C262" t="s">
         <v>6</v>
       </c>
+      <c r="D262">
+        <v>2006</v>
+      </c>
+      <c r="E262">
+        <v>-9.8654362810280602E-2</v>
+      </c>
       <c r="F262" t="s">
         <v>74</v>
       </c>
@@ -11250,6 +11988,12 @@
       <c r="C263" t="s">
         <v>6</v>
       </c>
+      <c r="D263">
+        <v>2007</v>
+      </c>
+      <c r="E263">
+        <v>-0.120603648768404</v>
+      </c>
       <c r="F263" t="s">
         <v>74</v>
       </c>
@@ -11285,6 +12029,12 @@
       <c r="C264" t="s">
         <v>6</v>
       </c>
+      <c r="D264">
+        <v>2008</v>
+      </c>
+      <c r="E264">
+        <v>-9.8640925744026303E-2</v>
+      </c>
       <c r="F264" t="s">
         <v>74</v>
       </c>
@@ -11320,6 +12070,12 @@
       <c r="C265" t="s">
         <v>6</v>
       </c>
+      <c r="D265">
+        <v>2009</v>
+      </c>
+      <c r="E265">
+        <v>-0.110520728544355</v>
+      </c>
       <c r="F265" t="s">
         <v>74</v>
       </c>
@@ -11355,6 +12111,12 @@
       <c r="C266" t="s">
         <v>6</v>
       </c>
+      <c r="D266">
+        <v>2010</v>
+      </c>
+      <c r="E266">
+        <v>-0.12399371931145101</v>
+      </c>
       <c r="F266" t="s">
         <v>74</v>
       </c>
@@ -11390,6 +12152,12 @@
       <c r="C267" t="s">
         <v>6</v>
       </c>
+      <c r="D267">
+        <v>2011</v>
+      </c>
+      <c r="E267">
+        <v>-0.104454872475764</v>
+      </c>
       <c r="F267" t="s">
         <v>74</v>
       </c>
@@ -11425,6 +12193,12 @@
       <c r="C268" t="s">
         <v>6</v>
       </c>
+      <c r="D268">
+        <v>2012</v>
+      </c>
+      <c r="E268">
+        <v>-9.8114465112108404E-2</v>
+      </c>
       <c r="F268" t="s">
         <v>74</v>
       </c>
@@ -11460,6 +12234,12 @@
       <c r="C269" t="s">
         <v>6</v>
       </c>
+      <c r="D269">
+        <v>2013</v>
+      </c>
+      <c r="E269">
+        <v>-0.116687277125042</v>
+      </c>
       <c r="F269" t="s">
         <v>74</v>
       </c>
@@ -11495,6 +12275,12 @@
       <c r="C270" t="s">
         <v>6</v>
       </c>
+      <c r="D270">
+        <v>2014</v>
+      </c>
+      <c r="E270">
+        <v>-0.104974559475654</v>
+      </c>
       <c r="F270" t="s">
         <v>74</v>
       </c>
@@ -11530,6 +12316,12 @@
       <c r="C271" t="s">
         <v>6</v>
       </c>
+      <c r="D271">
+        <v>2015</v>
+      </c>
+      <c r="E271">
+        <v>-9.6167998394552798E-2</v>
+      </c>
       <c r="F271" t="s">
         <v>74</v>
       </c>
@@ -11565,6 +12357,12 @@
       <c r="C272" t="s">
         <v>6</v>
       </c>
+      <c r="D272">
+        <v>2016</v>
+      </c>
+      <c r="E272">
+        <v>-9.1305139292434806E-2</v>
+      </c>
       <c r="F272" t="s">
         <v>74</v>
       </c>
@@ -11600,6 +12398,12 @@
       <c r="C273" t="s">
         <v>6</v>
       </c>
+      <c r="D273">
+        <v>2017</v>
+      </c>
+      <c r="E273">
+        <v>-0.104013253835956</v>
+      </c>
       <c r="F273" t="s">
         <v>74</v>
       </c>
@@ -11635,6 +12439,12 @@
       <c r="C274" t="s">
         <v>6</v>
       </c>
+      <c r="D274">
+        <v>2018</v>
+      </c>
+      <c r="E274">
+        <v>-0.1059191170285</v>
+      </c>
       <c r="F274" t="s">
         <v>74</v>
       </c>
@@ -11670,6 +12480,12 @@
       <c r="C275" t="s">
         <v>6</v>
       </c>
+      <c r="D275">
+        <v>2019</v>
+      </c>
+      <c r="E275">
+        <v>-0.11477451469956</v>
+      </c>
       <c r="F275" t="s">
         <v>74</v>
       </c>
@@ -11705,6 +12521,12 @@
       <c r="C276" t="s">
         <v>6</v>
       </c>
+      <c r="D276">
+        <v>2020</v>
+      </c>
+      <c r="E276">
+        <v>-0.11767116992299401</v>
+      </c>
       <c r="F276" t="s">
         <v>74</v>
       </c>
@@ -11740,6 +12562,12 @@
       <c r="C277" t="s">
         <v>6</v>
       </c>
+      <c r="D277">
+        <v>2021</v>
+      </c>
+      <c r="E277">
+        <v>-0.104036413674266</v>
+      </c>
       <c r="F277" t="s">
         <v>74</v>
       </c>
@@ -11775,6 +12603,12 @@
       <c r="C278" t="s">
         <v>6</v>
       </c>
+      <c r="D278">
+        <v>1999</v>
+      </c>
+      <c r="E278">
+        <v>-0.116245662438555</v>
+      </c>
       <c r="F278" t="s">
         <v>77</v>
       </c>
@@ -11810,6 +12644,12 @@
       <c r="C279" t="s">
         <v>6</v>
       </c>
+      <c r="D279">
+        <v>2000</v>
+      </c>
+      <c r="E279">
+        <v>-0.124021896437488</v>
+      </c>
       <c r="F279" t="s">
         <v>77</v>
       </c>
@@ -11845,6 +12685,12 @@
       <c r="C280" t="s">
         <v>6</v>
       </c>
+      <c r="D280">
+        <v>2001</v>
+      </c>
+      <c r="E280">
+        <v>-0.12800734793557</v>
+      </c>
       <c r="F280" t="s">
         <v>77</v>
       </c>
@@ -11880,6 +12726,12 @@
       <c r="C281" t="s">
         <v>6</v>
       </c>
+      <c r="D281">
+        <v>2002</v>
+      </c>
+      <c r="E281">
+        <v>-0.116478711743804</v>
+      </c>
       <c r="F281" t="s">
         <v>77</v>
       </c>
@@ -11915,6 +12767,12 @@
       <c r="C282" t="s">
         <v>6</v>
       </c>
+      <c r="D282">
+        <v>2003</v>
+      </c>
+      <c r="E282">
+        <v>-0.121845794238466</v>
+      </c>
       <c r="F282" t="s">
         <v>77</v>
       </c>
@@ -11950,6 +12808,12 @@
       <c r="C283" t="s">
         <v>6</v>
       </c>
+      <c r="D283">
+        <v>2004</v>
+      </c>
+      <c r="E283">
+        <v>-0.14374000170074699</v>
+      </c>
       <c r="F283" t="s">
         <v>77</v>
       </c>
@@ -11985,6 +12849,12 @@
       <c r="C284" t="s">
         <v>6</v>
       </c>
+      <c r="D284">
+        <v>2005</v>
+      </c>
+      <c r="E284">
+        <v>-0.13773898683535901</v>
+      </c>
       <c r="F284" t="s">
         <v>77</v>
       </c>
@@ -12020,6 +12890,12 @@
       <c r="C285" t="s">
         <v>6</v>
       </c>
+      <c r="D285">
+        <v>2006</v>
+      </c>
+      <c r="E285">
+        <v>-0.128145881047976</v>
+      </c>
       <c r="F285" t="s">
         <v>77</v>
       </c>
@@ -12055,6 +12931,12 @@
       <c r="C286" t="s">
         <v>6</v>
       </c>
+      <c r="D286">
+        <v>2007</v>
+      </c>
+      <c r="E286">
+        <v>-0.13372315607448201</v>
+      </c>
       <c r="F286" t="s">
         <v>77</v>
       </c>
@@ -12090,6 +12972,12 @@
       <c r="C287" t="s">
         <v>6</v>
       </c>
+      <c r="D287">
+        <v>2008</v>
+      </c>
+      <c r="E287">
+        <v>-0.13579969873033801</v>
+      </c>
       <c r="F287" t="s">
         <v>77</v>
       </c>
@@ -12125,6 +13013,12 @@
       <c r="C288" t="s">
         <v>6</v>
       </c>
+      <c r="D288">
+        <v>2009</v>
+      </c>
+      <c r="E288">
+        <v>-0.139755888514978</v>
+      </c>
       <c r="F288" t="s">
         <v>77</v>
       </c>
@@ -12160,6 +13054,12 @@
       <c r="C289" t="s">
         <v>6</v>
       </c>
+      <c r="D289">
+        <v>2010</v>
+      </c>
+      <c r="E289">
+        <v>-0.141699768237597</v>
+      </c>
       <c r="F289" t="s">
         <v>77</v>
       </c>
@@ -12195,6 +13095,12 @@
       <c r="C290" t="s">
         <v>6</v>
       </c>
+      <c r="D290">
+        <v>2011</v>
+      </c>
+      <c r="E290">
+        <v>-0.13772565758821301</v>
+      </c>
       <c r="F290" t="s">
         <v>77</v>
       </c>
@@ -12230,6 +13136,12 @@
       <c r="C291" t="s">
         <v>6</v>
       </c>
+      <c r="D291">
+        <v>2012</v>
+      </c>
+      <c r="E291">
+        <v>-0.15180500872736499</v>
+      </c>
       <c r="F291" t="s">
         <v>77</v>
       </c>
@@ -12265,6 +13177,12 @@
       <c r="C292" t="s">
         <v>6</v>
       </c>
+      <c r="D292">
+        <v>2013</v>
+      </c>
+      <c r="E292">
+        <v>-0.12593562141591799</v>
+      </c>
       <c r="F292" t="s">
         <v>77</v>
       </c>
@@ -12300,6 +13218,12 @@
       <c r="C293" t="s">
         <v>6</v>
       </c>
+      <c r="D293">
+        <v>2014</v>
+      </c>
+      <c r="E293">
+        <v>-0.135218700764376</v>
+      </c>
       <c r="F293" t="s">
         <v>77</v>
       </c>
@@ -12335,6 +13259,12 @@
       <c r="C294" t="s">
         <v>6</v>
       </c>
+      <c r="D294">
+        <v>2015</v>
+      </c>
+      <c r="E294">
+        <v>-0.13334574890106601</v>
+      </c>
       <c r="F294" t="s">
         <v>77</v>
       </c>
@@ -12370,6 +13300,12 @@
       <c r="C295" t="s">
         <v>6</v>
       </c>
+      <c r="D295">
+        <v>2016</v>
+      </c>
+      <c r="E295">
+        <v>-0.13033524571555799</v>
+      </c>
       <c r="F295" t="s">
         <v>77</v>
       </c>
@@ -12405,6 +13341,12 @@
       <c r="C296" t="s">
         <v>6</v>
       </c>
+      <c r="D296">
+        <v>2017</v>
+      </c>
+      <c r="E296">
+        <v>-0.14414758986411699</v>
+      </c>
       <c r="F296" t="s">
         <v>77</v>
       </c>
@@ -12440,6 +13382,12 @@
       <c r="C297" t="s">
         <v>6</v>
       </c>
+      <c r="D297">
+        <v>2018</v>
+      </c>
+      <c r="E297">
+        <v>-0.12992576220655999</v>
+      </c>
       <c r="F297" t="s">
         <v>77</v>
       </c>
@@ -12475,6 +13423,12 @@
       <c r="C298" t="s">
         <v>6</v>
       </c>
+      <c r="D298">
+        <v>2019</v>
+      </c>
+      <c r="E298">
+        <v>-0.13421331053662899</v>
+      </c>
       <c r="F298" t="s">
         <v>77</v>
       </c>
@@ -12510,6 +13464,12 @@
       <c r="C299" t="s">
         <v>6</v>
       </c>
+      <c r="D299">
+        <v>2020</v>
+      </c>
+      <c r="E299">
+        <v>-0.12781846949403999</v>
+      </c>
       <c r="F299" t="s">
         <v>77</v>
       </c>
@@ -12545,6 +13505,12 @@
       <c r="C300" t="s">
         <v>6</v>
       </c>
+      <c r="D300">
+        <v>2021</v>
+      </c>
+      <c r="E300">
+        <v>-0.12981515894016099</v>
+      </c>
       <c r="F300" t="s">
         <v>77</v>
       </c>
@@ -12580,6 +13546,12 @@
       <c r="C301" t="s">
         <v>6</v>
       </c>
+      <c r="D301">
+        <v>1999</v>
+      </c>
+      <c r="E301">
+        <v>-9.2875380752175205E-2</v>
+      </c>
       <c r="F301" t="s">
         <v>75</v>
       </c>
@@ -12615,6 +13587,12 @@
       <c r="C302" t="s">
         <v>6</v>
       </c>
+      <c r="D302">
+        <v>2000</v>
+      </c>
+      <c r="E302">
+        <v>-9.0773029647059106E-2</v>
+      </c>
       <c r="F302" t="s">
         <v>75</v>
       </c>
@@ -12650,6 +13628,12 @@
       <c r="C303" t="s">
         <v>6</v>
       </c>
+      <c r="D303">
+        <v>2001</v>
+      </c>
+      <c r="E303">
+        <v>-9.6539692667231294E-2</v>
+      </c>
       <c r="F303" t="s">
         <v>75</v>
       </c>
@@ -12685,6 +13669,12 @@
       <c r="C304" t="s">
         <v>6</v>
       </c>
+      <c r="D304">
+        <v>2002</v>
+      </c>
+      <c r="E304">
+        <v>-9.0799205893971294E-2</v>
+      </c>
       <c r="F304" t="s">
         <v>75</v>
       </c>
@@ -12720,6 +13710,12 @@
       <c r="C305" t="s">
         <v>6</v>
       </c>
+      <c r="D305">
+        <v>2003</v>
+      </c>
+      <c r="E305">
+        <v>-0.100696804021354</v>
+      </c>
       <c r="F305" t="s">
         <v>75</v>
       </c>
@@ -12755,6 +13751,12 @@
       <c r="C306" t="s">
         <v>6</v>
       </c>
+      <c r="D306">
+        <v>2004</v>
+      </c>
+      <c r="E306">
+        <v>-0.10846283359379599</v>
+      </c>
       <c r="F306" t="s">
         <v>75</v>
       </c>
@@ -12790,6 +13792,12 @@
       <c r="C307" t="s">
         <v>6</v>
       </c>
+      <c r="D307">
+        <v>2005</v>
+      </c>
+      <c r="E307">
+        <v>-0.10444773790242</v>
+      </c>
       <c r="F307" t="s">
         <v>75</v>
       </c>
@@ -12825,6 +13833,12 @@
       <c r="C308" t="s">
         <v>6</v>
       </c>
+      <c r="D308">
+        <v>2006</v>
+      </c>
+      <c r="E308">
+        <v>-0.10453338722185</v>
+      </c>
       <c r="F308" t="s">
         <v>75</v>
       </c>
@@ -12860,6 +13874,12 @@
       <c r="C309" t="s">
         <v>6</v>
       </c>
+      <c r="D309">
+        <v>2007</v>
+      </c>
+      <c r="E309">
+        <v>-9.8597068304503294E-2</v>
+      </c>
       <c r="F309" t="s">
         <v>75</v>
       </c>
@@ -12895,6 +13915,12 @@
       <c r="C310" t="s">
         <v>6</v>
       </c>
+      <c r="D310">
+        <v>2008</v>
+      </c>
+      <c r="E310">
+        <v>-0.10839930719425001</v>
+      </c>
       <c r="F310" t="s">
         <v>75</v>
       </c>
@@ -12930,6 +13956,12 @@
       <c r="C311" t="s">
         <v>6</v>
       </c>
+      <c r="D311">
+        <v>2009</v>
+      </c>
+      <c r="E311">
+        <v>-0.100550193368941</v>
+      </c>
       <c r="F311" t="s">
         <v>75</v>
       </c>
@@ -12965,6 +13997,12 @@
       <c r="C312" t="s">
         <v>6</v>
       </c>
+      <c r="D312">
+        <v>2010</v>
+      </c>
+      <c r="E312">
+        <v>-0.10257872608603499</v>
+      </c>
       <c r="F312" t="s">
         <v>75</v>
       </c>
@@ -13000,6 +14038,12 @@
       <c r="C313" t="s">
         <v>6</v>
       </c>
+      <c r="D313">
+        <v>2011</v>
+      </c>
+      <c r="E313">
+        <v>-0.11916911694582299</v>
+      </c>
       <c r="F313" t="s">
         <v>75</v>
       </c>
@@ -13035,6 +14079,12 @@
       <c r="C314" t="s">
         <v>6</v>
       </c>
+      <c r="D314">
+        <v>2012</v>
+      </c>
+      <c r="E314">
+        <v>-0.104526658540568</v>
+      </c>
       <c r="F314" t="s">
         <v>75</v>
       </c>
@@ -13070,6 +14120,12 @@
       <c r="C315" t="s">
         <v>6</v>
       </c>
+      <c r="D315">
+        <v>2013</v>
+      </c>
+      <c r="E315">
+        <v>-9.6786698580918096E-2</v>
+      </c>
       <c r="F315" t="s">
         <v>75</v>
       </c>
@@ -13105,6 +14161,12 @@
       <c r="C316" t="s">
         <v>6</v>
       </c>
+      <c r="D316">
+        <v>2014</v>
+      </c>
+      <c r="E316">
+        <v>-9.6760755761570505E-2</v>
+      </c>
       <c r="F316" t="s">
         <v>75</v>
       </c>
@@ -13140,6 +14202,12 @@
       <c r="C317" t="s">
         <v>6</v>
       </c>
+      <c r="D317">
+        <v>2015</v>
+      </c>
+      <c r="E317">
+        <v>-9.8667592603635307E-2</v>
+      </c>
       <c r="F317" t="s">
         <v>75</v>
       </c>
@@ -13175,6 +14243,12 @@
       <c r="C318" t="s">
         <v>6</v>
       </c>
+      <c r="D318">
+        <v>2016</v>
+      </c>
+      <c r="E318">
+        <v>-9.4587770778986696E-2</v>
+      </c>
       <c r="F318" t="s">
         <v>75</v>
       </c>
@@ -13210,6 +14284,12 @@
       <c r="C319" t="s">
         <v>6</v>
       </c>
+      <c r="D319">
+        <v>2017</v>
+      </c>
+      <c r="E319">
+        <v>-0.11034359689892401</v>
+      </c>
       <c r="F319" t="s">
         <v>75</v>
       </c>
@@ -13245,6 +14325,12 @@
       <c r="C320" t="s">
         <v>6</v>
       </c>
+      <c r="D320">
+        <v>2018</v>
+      </c>
+      <c r="E320">
+        <v>-0.10245783664701399</v>
+      </c>
       <c r="F320" t="s">
         <v>75</v>
       </c>
@@ -13280,6 +14366,12 @@
       <c r="C321" t="s">
         <v>6</v>
       </c>
+      <c r="D321">
+        <v>2019</v>
+      </c>
+      <c r="E321">
+        <v>-8.6962897998755298E-2</v>
+      </c>
       <c r="F321" t="s">
         <v>75</v>
       </c>
@@ -13315,6 +14407,12 @@
       <c r="C322" t="s">
         <v>6</v>
       </c>
+      <c r="D322">
+        <v>2020</v>
+      </c>
+      <c r="E322">
+        <v>-9.8603037116614597E-2</v>
+      </c>
       <c r="F322" t="s">
         <v>75</v>
       </c>
@@ -13350,6 +14448,12 @@
       <c r="C323" t="s">
         <v>6</v>
       </c>
+      <c r="D323">
+        <v>2021</v>
+      </c>
+      <c r="E323">
+        <v>-9.2674171892042495E-2</v>
+      </c>
       <c r="F323" t="s">
         <v>75</v>
       </c>
@@ -13385,6 +14489,12 @@
       <c r="C324" t="s">
         <v>6</v>
       </c>
+      <c r="D324">
+        <v>1999</v>
+      </c>
+      <c r="E324">
+        <v>-6.9362730374295398E-2</v>
+      </c>
       <c r="F324" t="s">
         <v>77</v>
       </c>
@@ -13420,6 +14530,12 @@
       <c r="C325" t="s">
         <v>6</v>
       </c>
+      <c r="D325">
+        <v>2000</v>
+      </c>
+      <c r="E325">
+        <v>-7.3108653586986497E-2</v>
+      </c>
       <c r="F325" t="s">
         <v>77</v>
       </c>
@@ -13455,6 +14571,12 @@
       <c r="C326" t="s">
         <v>6</v>
       </c>
+      <c r="D326">
+        <v>2001</v>
+      </c>
+      <c r="E326">
+        <v>-7.1324032100691701E-2</v>
+      </c>
       <c r="F326" t="s">
         <v>77</v>
       </c>
@@ -13490,6 +14612,12 @@
       <c r="C327" t="s">
         <v>6</v>
       </c>
+      <c r="D327">
+        <v>2002</v>
+      </c>
+      <c r="E327">
+        <v>-6.5413246070240599E-2</v>
+      </c>
       <c r="F327" t="s">
         <v>77</v>
       </c>
@@ -13525,6 +14653,12 @@
       <c r="C328" t="s">
         <v>6</v>
       </c>
+      <c r="D328">
+        <v>2003</v>
+      </c>
+      <c r="E328">
+        <v>-8.10307981485512E-2</v>
+      </c>
       <c r="F328" t="s">
         <v>77</v>
       </c>
@@ -13560,6 +14694,12 @@
       <c r="C329" t="s">
         <v>6</v>
       </c>
+      <c r="D329">
+        <v>2004</v>
+      </c>
+      <c r="E329">
+        <v>-7.9077302386796E-2</v>
+      </c>
       <c r="F329" t="s">
         <v>77</v>
       </c>
@@ -13595,6 +14735,12 @@
       <c r="C330" t="s">
         <v>6</v>
       </c>
+      <c r="D330">
+        <v>2005</v>
+      </c>
+      <c r="E330">
+        <v>-8.1003246856190106E-2</v>
+      </c>
       <c r="F330" t="s">
         <v>77</v>
       </c>
@@ -13630,6 +14776,12 @@
       <c r="C331" t="s">
         <v>6</v>
       </c>
+      <c r="D331">
+        <v>2006</v>
+      </c>
+      <c r="E331">
+        <v>-8.1030980083363999E-2</v>
+      </c>
       <c r="F331" t="s">
         <v>77</v>
       </c>
@@ -13665,6 +14817,12 @@
       <c r="C332" t="s">
         <v>6</v>
       </c>
+      <c r="D332">
+        <v>2007</v>
+      </c>
+      <c r="E332">
+        <v>-7.1268448335076395E-2</v>
+      </c>
       <c r="F332" t="s">
         <v>77</v>
       </c>
@@ -13700,6 +14858,12 @@
       <c r="C333" t="s">
         <v>6</v>
       </c>
+      <c r="D333">
+        <v>2008</v>
+      </c>
+      <c r="E333">
+        <v>-7.3221955559263599E-2</v>
+      </c>
       <c r="F333" t="s">
         <v>77</v>
       </c>
@@ -13735,6 +14899,12 @@
       <c r="C334" t="s">
         <v>6</v>
       </c>
+      <c r="D334">
+        <v>2009</v>
+      </c>
+      <c r="E334">
+        <v>-7.7185578871551003E-2</v>
+      </c>
       <c r="F334" t="s">
         <v>77</v>
       </c>
@@ -13770,6 +14940,12 @@
       <c r="C335" t="s">
         <v>6</v>
       </c>
+      <c r="D335">
+        <v>2010</v>
+      </c>
+      <c r="E335">
+        <v>-7.9148557375370701E-2</v>
+      </c>
       <c r="F335" t="s">
         <v>77</v>
       </c>
@@ -13805,6 +14981,12 @@
       <c r="C336" t="s">
         <v>6</v>
       </c>
+      <c r="D336">
+        <v>2011</v>
+      </c>
+      <c r="E336">
+        <v>-7.5201119250214402E-2</v>
+      </c>
       <c r="F336" t="s">
         <v>77</v>
       </c>
@@ -13840,6 +15022,12 @@
       <c r="C337" t="s">
         <v>6</v>
       </c>
+      <c r="D337">
+        <v>2012</v>
+      </c>
+      <c r="E337">
+        <v>-7.13122802390182E-2</v>
+      </c>
       <c r="F337" t="s">
         <v>77</v>
       </c>
@@ -13875,6 +15063,12 @@
       <c r="C338" t="s">
         <v>6</v>
       </c>
+      <c r="D338">
+        <v>2013</v>
+      </c>
+      <c r="E338">
+        <v>-7.5166977844770305E-2</v>
+      </c>
       <c r="F338" t="s">
         <v>77</v>
       </c>
@@ -13910,6 +15104,12 @@
       <c r="C339" t="s">
         <v>6</v>
       </c>
+      <c r="D339">
+        <v>2014</v>
+      </c>
+      <c r="E339">
+        <v>-8.0995928137107195E-2</v>
+      </c>
       <c r="F339" t="s">
         <v>77</v>
       </c>
@@ -13945,6 +15145,12 @@
       <c r="C340" t="s">
         <v>6</v>
       </c>
+      <c r="D340">
+        <v>2015</v>
+      </c>
+      <c r="E340">
+        <v>-7.5123205242623101E-2</v>
+      </c>
       <c r="F340" t="s">
         <v>77</v>
       </c>
@@ -13980,6 +15186,12 @@
       <c r="C341" t="s">
         <v>6</v>
       </c>
+      <c r="D341">
+        <v>2016</v>
+      </c>
+      <c r="E341">
+        <v>-7.9102863493754602E-2</v>
+      </c>
       <c r="F341" t="s">
         <v>77</v>
       </c>
@@ -14015,6 +15227,12 @@
       <c r="C342" t="s">
         <v>6</v>
       </c>
+      <c r="D342">
+        <v>2017</v>
+      </c>
+      <c r="E342">
+        <v>-7.3172526296126306E-2</v>
+      </c>
       <c r="F342" t="s">
         <v>77</v>
       </c>
@@ -14050,6 +15268,12 @@
       <c r="C343" t="s">
         <v>6</v>
       </c>
+      <c r="D343">
+        <v>2018</v>
+      </c>
+      <c r="E343">
+        <v>-7.5192102511495607E-2</v>
+      </c>
       <c r="F343" t="s">
         <v>77</v>
       </c>
@@ -14085,6 +15309,12 @@
       <c r="C344" t="s">
         <v>6</v>
       </c>
+      <c r="D344">
+        <v>2019</v>
+      </c>
+      <c r="E344">
+        <v>-7.5234326074674507E-2</v>
+      </c>
       <c r="F344" t="s">
         <v>77</v>
       </c>
@@ -14120,6 +15350,12 @@
       <c r="C345" t="s">
         <v>6</v>
       </c>
+      <c r="D345">
+        <v>2020</v>
+      </c>
+      <c r="E345">
+        <v>-7.3329343445437803E-2</v>
+      </c>
       <c r="F345" t="s">
         <v>77</v>
       </c>
@@ -14154,6 +15390,12 @@
       </c>
       <c r="C346" t="s">
         <v>6</v>
+      </c>
+      <c r="D346">
+        <v>2021</v>
+      </c>
+      <c r="E346">
+        <v>-6.9315128017360797E-2</v>
       </c>
       <c r="F346" t="s">
         <v>77</v>

</xml_diff>